<commit_message>
uploading jar and source files
</commit_message>
<xml_diff>
--- a/util-projects/java-utility-parent/excel-yaml-utility/src/main/resources/excelFile.xlsx
+++ b/util-projects/java-utility-parent/excel-yaml-utility/src/main/resources/excelFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Storage\workspace\java\mycode\java-util-projects\util-projects\java-utility-parent\excel-yaml-utility\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\excelToYaml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181C05A6-1A81-4C39-AF9E-69B4BAB49EC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90244994-3FD8-4EDF-AE94-74B0AB159D21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{12A38895-378F-4CD7-9819-0CE949D0A229}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{12A38895-378F-4CD7-9819-0CE949D0A229}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>S.No</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>$ref</t>
+  </si>
+  <si>
+    <t>phone.yaml</t>
   </si>
 </sst>
 </file>
@@ -222,10 +231,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -541,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC35002-9CDC-416E-B1B0-6AC6A9264308}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,10 +566,11 @@
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,8 +598,11 @@
       <c r="I1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -611,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -634,7 +648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -660,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -689,7 +703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -718,30 +732,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7">
-        <v>2342512354</v>
-      </c>
       <c r="I7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -760,8 +768,11 @@
       <c r="I8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -781,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -801,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -821,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -841,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -861,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -879,6 +890,32 @@
       </c>
       <c r="I14" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>342342</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>